<commit_message>
very close to original JRC results now
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_NODESTEC.xlsx
+++ b/SuppXLS/Scen_NODESTEC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NewVEDA\Veda_models\EU_TIMES_Veda2.0\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA15D254-49E5-4590-8BCC-B9E8F9FC110E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D485B4-99C7-4185-988E-A319DC74CD09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INS" sheetId="2" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Pset_CI</t>
   </si>
@@ -131,9 +131,6 @@
   </si>
   <si>
     <t>IMPELC-DESTEC</t>
-  </si>
-  <si>
-    <t>EUWINOFV01</t>
   </si>
 </sst>
 </file>
@@ -583,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,17 +680,6 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5">
-        <v>2100</v>
-      </c>
-      <c r="J5" t="s">
-        <v>19</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>